<commit_message>
Updated tables - added tested parameters
</commit_message>
<xml_diff>
--- a/analysis/bioenv_results.xlsx
+++ b/analysis/bioenv_results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="39">
   <si>
     <t>Laurentian (n = 35)</t>
   </si>
@@ -36,33 +36,21 @@
     <t>Whole Community</t>
   </si>
   <si>
-    <t>Best predictor(s)</t>
-  </si>
-  <si>
     <t>DO</t>
   </si>
   <si>
     <t>0.445 (0.01*)</t>
   </si>
   <si>
-    <t>0.375 (0.01**)</t>
-  </si>
-  <si>
     <t>0.179 (0.01**)</t>
   </si>
   <si>
     <t>0.551 (0.01**)</t>
   </si>
   <si>
-    <t>0.455 (0.01**)</t>
-  </si>
-  <si>
     <t>PP</t>
   </si>
   <si>
-    <t>TDP-SRP</t>
-  </si>
-  <si>
     <t>PAR</t>
   </si>
   <si>
@@ -88,6 +76,66 @@
   </si>
   <si>
     <t xml:space="preserve"> Correlation</t>
+  </si>
+  <si>
+    <t>Tested parameters</t>
+  </si>
+  <si>
+    <t>Best parameters(s)</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>0.443 (0.01**)</t>
+  </si>
+  <si>
+    <t>POC</t>
+  </si>
+  <si>
+    <t>PON</t>
+  </si>
+  <si>
+    <t>DOC</t>
+  </si>
+  <si>
+    <t>SiO2</t>
+  </si>
+  <si>
+    <t>TSS</t>
+  </si>
+  <si>
+    <t>Fluorescence</t>
+  </si>
+  <si>
+    <t>TDS</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>ORP</t>
+  </si>
+  <si>
+    <t>Cl</t>
+  </si>
+  <si>
+    <t>BGA</t>
+  </si>
+  <si>
+    <t>SO4</t>
+  </si>
+  <si>
+    <t>TKN</t>
+  </si>
+  <si>
+    <t>0.373 (0.01**)</t>
+  </si>
+  <si>
+    <t>Turbidity</t>
+  </si>
+  <si>
+    <t>Alkalinity</t>
   </si>
 </sst>
 </file>
@@ -97,7 +145,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -135,6 +183,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -144,7 +199,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -255,13 +310,87 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -276,12 +405,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -305,10 +428,90 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -638,15 +841,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="I4" sqref="I4:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
@@ -655,165 +858,466 @@
     <col min="7" max="7" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="1:9">
+      <c r="B1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="8" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="24"/>
+      <c r="F1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="9"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="B2" s="14" t="s">
+      <c r="G1" s="24"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="B2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:9">
+      <c r="A3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="C4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="40"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="40"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="40"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="40"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="36"/>
+      <c r="G9" s="32"/>
+      <c r="I9" s="40"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="36"/>
+      <c r="G10" s="32"/>
+      <c r="I10" s="40"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="36"/>
+      <c r="G11" s="32"/>
+      <c r="I11" s="40"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="36"/>
+      <c r="G12" s="32"/>
+      <c r="I12" s="40"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="36"/>
+      <c r="G13" s="32"/>
+      <c r="I13" s="40"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="36"/>
+      <c r="G14" s="32"/>
+      <c r="I14" s="40"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="36"/>
+      <c r="G15" s="32"/>
+      <c r="I15" s="40"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="36"/>
+      <c r="G16" s="32"/>
+      <c r="I16" s="40"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="36"/>
+      <c r="G17" s="32"/>
+      <c r="I17" s="40"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="37"/>
+      <c r="G18" s="33"/>
+      <c r="I18" s="40"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="40"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="10"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="40"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="10"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="40"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="11"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="40"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="22">
+        <v>0.125</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="12"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="12"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="13"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="24" t="s">
+      <c r="G23" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="24">
-        <v>0.125</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="3"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="I23" s="40"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="3"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>